<commit_message>
System to copy files to dropbox
</commit_message>
<xml_diff>
--- a/clean_data/ERP_projects.xlsx
+++ b/clean_data/ERP_projects.xlsx
@@ -222,10 +222,10 @@
     <t>date_start</t>
   </si>
   <si>
-    <t>date_until</t>
-  </si>
-  <si>
-    <t>date_end</t>
+    <t>date_actual_todate</t>
+  </si>
+  <si>
+    <t>date_close</t>
   </si>
   <si>
     <t>Months</t>
@@ -2125,10 +2125,10 @@
         <v>58</v>
       </c>
       <c r="F2" s="0">
-        <v>1486798.375</v>
+        <v>1877033.75</v>
       </c>
       <c r="G2" s="0">
-        <v>651852.9375</v>
+        <v>822942.6875</v>
       </c>
       <c r="H2" s="0">
         <v>0.43999999761581421</v>
@@ -2146,34 +2146,34 @@
         <v>48.919998168945313</v>
       </c>
       <c r="M2" s="0">
-        <v>13324.876953125</v>
+        <v>16822.21484375</v>
       </c>
       <c r="N2" s="0">
         <v>4</v>
       </c>
       <c r="O2" s="0">
-        <v>53299.5078125</v>
+        <v>67288.859375</v>
       </c>
       <c r="P2" s="0">
         <v>4</v>
       </c>
       <c r="Q2" s="0">
-        <v>53299.5078125</v>
+        <v>67288.859375</v>
       </c>
       <c r="R2" s="0">
         <v>12</v>
       </c>
       <c r="S2" s="0">
-        <v>159898.53125</v>
+        <v>201866.578125</v>
       </c>
       <c r="T2" s="0">
         <v>12</v>
       </c>
       <c r="U2" s="0">
-        <v>159898.53125</v>
+        <v>201866.578125</v>
       </c>
       <c r="V2" s="0">
-        <v>373096.5625</v>
+        <v>471022</v>
       </c>
       <c r="W2" s="0">
         <v>1</v>
@@ -2194,19 +2194,19 @@
         <v>1</v>
       </c>
       <c r="AC2" s="0">
-        <v>373096.5625</v>
+        <v>471022</v>
       </c>
       <c r="AD2" s="0">
         <v>0.85000002384185791</v>
       </c>
       <c r="AE2" s="0">
-        <v>317132.09375</v>
+        <v>400368.71875</v>
       </c>
       <c r="AF2" s="0">
         <v>0.34999999403953552</v>
       </c>
       <c r="AG2" s="0">
-        <v>130583.796875</v>
+        <v>164857.703125</v>
       </c>
       <c r="AH2" s="0">
         <v>0.40000000596046448</v>
@@ -2222,56 +2222,56 @@
         <v>1</v>
       </c>
       <c r="AM2" s="0">
-        <v>126852.8359375</v>
+        <v>160147.484375</v>
       </c>
       <c r="AN2" s="0">
-        <v>110996.234375</v>
+        <v>140129.046875</v>
       </c>
       <c r="AO2" s="0">
-        <v>79283.0234375</v>
+        <v>100092.1796875</v>
       </c>
       <c r="AP2" s="0"/>
       <c r="AQ2" s="0"/>
       <c r="AR2" s="0">
-        <v>110996.234375</v>
+        <v>140129.046875</v>
       </c>
       <c r="AS2" s="0">
-        <v>15856.6044921875</v>
+        <v>20018.435546875</v>
       </c>
       <c r="AT2" s="0">
-        <v>110996.234375</v>
+        <v>140129.046875</v>
       </c>
       <c r="AU2" s="0">
-        <v>15856.6044921875</v>
+        <v>20018.435546875</v>
       </c>
       <c r="AV2" s="0">
-        <v>63426.41796875</v>
+        <v>80073.7421875</v>
       </c>
       <c r="AW2" s="0"/>
       <c r="AX2" s="0"/>
       <c r="AY2" s="0">
-        <v>31713.208984375</v>
+        <v>40036.87109375</v>
       </c>
       <c r="AZ2" s="0">
-        <v>63426.41796875</v>
+        <v>80073.7421875</v>
       </c>
       <c r="BA2" s="0">
-        <v>79283.0234375</v>
+        <v>100092.1796875</v>
       </c>
       <c r="BB2" s="0">
-        <v>47569.81640625</v>
+        <v>60055.30859375</v>
       </c>
       <c r="BC2" s="0">
-        <v>31713.208984375</v>
+        <v>40036.87109375</v>
       </c>
       <c r="BD2" s="0">
-        <v>31713.208984375</v>
+        <v>40036.87109375</v>
       </c>
       <c r="BE2" s="0">
-        <v>15856.6044921875</v>
+        <v>20018.435546875</v>
       </c>
       <c r="BF2" s="0">
-        <v>15856.6044921875</v>
+        <v>20018.435546875</v>
       </c>
       <c r="BG2" s="0"/>
       <c r="BH2" s="0"/>
@@ -2360,7 +2360,7 @@
         <v>479</v>
       </c>
       <c r="CM2" s="0">
-        <v>317132.09375</v>
+        <v>400368.71875</v>
       </c>
       <c r="CN2" s="0">
         <v>0</v>
@@ -2383,10 +2383,10 @@
         <v>58</v>
       </c>
       <c r="F3" s="0">
-        <v>1780000</v>
+        <v>2247191</v>
       </c>
       <c r="G3" s="0">
-        <v>1780000</v>
+        <v>2247191</v>
       </c>
       <c r="H3" s="0">
         <v>1</v>
@@ -2404,34 +2404,34 @@
         <v>24.989999771118164</v>
       </c>
       <c r="M3" s="0">
-        <v>71228.4921875</v>
+        <v>89923.609375</v>
       </c>
       <c r="N3" s="0">
         <v>6.9000000953674316</v>
       </c>
       <c r="O3" s="0">
-        <v>491476.59375</v>
+        <v>620472.9375</v>
       </c>
       <c r="P3" s="0">
         <v>6.9000000953674316</v>
       </c>
       <c r="Q3" s="0">
-        <v>491476.59375</v>
+        <v>620472.9375</v>
       </c>
       <c r="R3" s="0">
         <v>12</v>
       </c>
       <c r="S3" s="0">
-        <v>854741.875</v>
+        <v>1079083.25</v>
       </c>
       <c r="T3" s="0">
         <v>12</v>
       </c>
       <c r="U3" s="0">
-        <v>854741.875</v>
+        <v>1079083.25</v>
       </c>
       <c r="V3" s="0">
-        <v>2200960.5</v>
+        <v>2778639.5</v>
       </c>
       <c r="W3" s="0">
         <v>1</v>
@@ -2452,13 +2452,13 @@
         <v>1</v>
       </c>
       <c r="AC3" s="0">
-        <v>2200960.5</v>
+        <v>2778639.5</v>
       </c>
       <c r="AD3" s="0">
         <v>1</v>
       </c>
       <c r="AE3" s="0">
-        <v>2200960.5</v>
+        <v>2778639.5</v>
       </c>
       <c r="AF3" s="0"/>
       <c r="AG3" s="0"/>
@@ -2475,21 +2475,21 @@
       <c r="AN3" s="0"/>
       <c r="AO3" s="0"/>
       <c r="AP3" s="0">
-        <v>2200960.5</v>
+        <v>2778639.5</v>
       </c>
       <c r="AQ3" s="0"/>
       <c r="AR3" s="0"/>
       <c r="AS3" s="0"/>
       <c r="AT3" s="0"/>
       <c r="AU3" s="0">
-        <v>1980864.375</v>
+        <v>2500775.5</v>
       </c>
       <c r="AV3" s="0"/>
       <c r="AW3" s="0">
-        <v>220096.046875</v>
+        <v>277863.96875</v>
       </c>
       <c r="AX3" s="0">
-        <v>220096.046875</v>
+        <v>277863.96875</v>
       </c>
       <c r="AY3" s="0"/>
       <c r="AZ3" s="0"/>
@@ -2497,12 +2497,12 @@
       <c r="BB3" s="0"/>
       <c r="BC3" s="0"/>
       <c r="BD3" s="0">
-        <v>220096.046875</v>
+        <v>277863.96875</v>
       </c>
       <c r="BE3" s="0"/>
       <c r="BF3" s="0"/>
       <c r="BG3" s="0">
-        <v>1760768.375</v>
+        <v>2222911.75</v>
       </c>
       <c r="BH3" s="0"/>
       <c r="BI3" s="0"/>
@@ -2574,7 +2574,7 @@
         <v>62</v>
       </c>
       <c r="CM3" s="0">
-        <v>2200960.5</v>
+        <v>2778639.5</v>
       </c>
       <c r="CN3" s="0">
         <v>0</v>
@@ -3597,13 +3597,13 @@
         <v>60</v>
       </c>
       <c r="F8" s="0">
-        <v>336267.8125</v>
+        <v>424526.96875</v>
       </c>
       <c r="G8" s="0">
         <v>392018.3125</v>
       </c>
       <c r="H8" s="0">
-        <v>1.1699999570846558</v>
+        <v>0.92000001668930054</v>
       </c>
       <c r="I8" s="1">
         <v>42856</v>
@@ -4835,7 +4835,7 @@
       <c r="T13" s="0"/>
       <c r="U13" s="0"/>
       <c r="V13" s="0">
-        <v>1290309.5</v>
+        <v>574774.25</v>
       </c>
       <c r="W13" s="0">
         <v>1</v>
@@ -4856,13 +4856,13 @@
         <v>1</v>
       </c>
       <c r="AC13" s="0">
-        <v>1290309.5</v>
+        <v>574774.25</v>
       </c>
       <c r="AD13" s="0">
         <v>1</v>
       </c>
       <c r="AE13" s="0">
-        <v>1290309.5</v>
+        <v>574774.25</v>
       </c>
       <c r="AF13" s="0">
         <v>0</v>
@@ -4884,35 +4884,35 @@
         <v>1</v>
       </c>
       <c r="AM13" s="0">
-        <v>645154.75</v>
+        <v>287387.125</v>
       </c>
       <c r="AN13" s="0">
-        <v>322577.375</v>
+        <v>143693.5625</v>
       </c>
       <c r="AO13" s="0">
-        <v>322577.375</v>
+        <v>143693.5625</v>
       </c>
       <c r="AP13" s="0"/>
       <c r="AQ13" s="0"/>
       <c r="AR13" s="0">
-        <v>774185.75</v>
+        <v>344864.5625</v>
       </c>
       <c r="AS13" s="0">
-        <v>516123.8125</v>
+        <v>229909.703125</v>
       </c>
       <c r="AT13" s="0"/>
       <c r="AU13" s="0"/>
       <c r="AV13" s="0"/>
       <c r="AW13" s="0"/>
       <c r="AX13" s="0">
-        <v>322577.375</v>
+        <v>143693.5625</v>
       </c>
       <c r="AY13" s="0">
-        <v>322577.375</v>
+        <v>143693.5625</v>
       </c>
       <c r="AZ13" s="0"/>
       <c r="BA13" s="0">
-        <v>322577.375</v>
+        <v>143693.5625</v>
       </c>
       <c r="BB13" s="0"/>
       <c r="BC13" s="0"/>
@@ -4920,7 +4920,7 @@
       <c r="BE13" s="0"/>
       <c r="BF13" s="0"/>
       <c r="BG13" s="0">
-        <v>322577.375</v>
+        <v>143693.5625</v>
       </c>
       <c r="BH13" s="0"/>
       <c r="BI13" s="0">
@@ -4994,7 +4994,7 @@
         <v>62</v>
       </c>
       <c r="CM13" s="0">
-        <v>1290309.5</v>
+        <v>574774.25</v>
       </c>
       <c r="CN13" s="0">
         <v>0</v>
@@ -5517,10 +5517,10 @@
         <v>58</v>
       </c>
       <c r="F16" s="0">
-        <v>623000</v>
+        <v>786516.875</v>
       </c>
       <c r="G16" s="0">
-        <v>623000</v>
+        <v>786516.875</v>
       </c>
       <c r="H16" s="0">
         <v>1</v>
@@ -5538,26 +5538,26 @@
         <v>11.970000267028809</v>
       </c>
       <c r="M16" s="0">
-        <v>52046.78125</v>
+        <v>65707.3359375</v>
       </c>
       <c r="N16" s="0">
         <v>2.9000000953674316</v>
       </c>
       <c r="O16" s="0">
-        <v>150935.671875</v>
+        <v>190551.28125</v>
       </c>
       <c r="P16" s="0">
         <v>9</v>
       </c>
       <c r="Q16" s="0">
-        <v>468421.03125</v>
+        <v>591366</v>
       </c>
       <c r="R16" s="0"/>
       <c r="S16" s="0"/>
       <c r="T16" s="0"/>
       <c r="U16" s="0"/>
       <c r="V16" s="0">
-        <v>468421.03125</v>
+        <v>190551.28125</v>
       </c>
       <c r="W16" s="0">
         <v>2</v>
@@ -5576,13 +5576,13 @@
         <v>1</v>
       </c>
       <c r="AC16" s="0">
-        <v>468421.03125</v>
+        <v>190551.28125</v>
       </c>
       <c r="AD16" s="0">
         <v>1</v>
       </c>
       <c r="AE16" s="0">
-        <v>468421.03125</v>
+        <v>190551.28125</v>
       </c>
       <c r="AF16" s="0">
         <v>0</v>
@@ -5606,46 +5606,46 @@
         <v>0.99999994039535522</v>
       </c>
       <c r="AM16" s="0">
-        <v>304473.65625</v>
+        <v>123858.328125</v>
       </c>
       <c r="AN16" s="0">
-        <v>70263.15625</v>
+        <v>28582.693359375</v>
       </c>
       <c r="AO16" s="0">
-        <v>93684.2109375</v>
+        <v>38110.2578125</v>
       </c>
       <c r="AP16" s="0">
         <v>0</v>
       </c>
       <c r="AQ16" s="0"/>
       <c r="AR16" s="0">
-        <v>374736.84375</v>
+        <v>152441.03125</v>
       </c>
       <c r="AS16" s="0"/>
       <c r="AT16" s="0"/>
       <c r="AU16" s="0"/>
       <c r="AV16" s="0">
-        <v>46842.10546875</v>
+        <v>19055.12890625</v>
       </c>
       <c r="AW16" s="0">
-        <v>46842.10546875</v>
+        <v>19055.12890625</v>
       </c>
       <c r="AX16" s="0">
-        <v>234210.515625</v>
+        <v>95275.640625</v>
       </c>
       <c r="AY16" s="0">
-        <v>70263.15625</v>
+        <v>28582.693359375</v>
       </c>
       <c r="AZ16" s="0"/>
       <c r="BA16" s="0">
-        <v>70263.15625</v>
+        <v>28582.693359375</v>
       </c>
       <c r="BB16" s="0"/>
       <c r="BC16" s="0">
-        <v>46842.10546875</v>
+        <v>19055.12890625</v>
       </c>
       <c r="BD16" s="0">
-        <v>46842.10546875</v>
+        <v>19055.12890625</v>
       </c>
       <c r="BE16" s="0"/>
       <c r="BF16" s="0"/>
@@ -5726,7 +5726,7 @@
         <v>62</v>
       </c>
       <c r="CM16" s="0">
-        <v>468421.03125</v>
+        <v>190551.28125</v>
       </c>
       <c r="CN16" s="0">
         <v>0</v>
@@ -5749,10 +5749,10 @@
         <v>58</v>
       </c>
       <c r="F17" s="0">
-        <v>596300</v>
+        <v>752809</v>
       </c>
       <c r="G17" s="0">
-        <v>596300</v>
+        <v>752809</v>
       </c>
       <c r="H17" s="0">
         <v>1</v>
@@ -5770,30 +5770,30 @@
         <v>11.970000267028809</v>
       </c>
       <c r="M17" s="0">
-        <v>49816.20703125</v>
+        <v>62891.30859375</v>
       </c>
       <c r="N17" s="0">
         <v>3</v>
       </c>
       <c r="O17" s="0">
-        <v>149448.625</v>
+        <v>188673.921875</v>
       </c>
       <c r="P17" s="0">
         <v>3</v>
       </c>
       <c r="Q17" s="0">
-        <v>149448.625</v>
+        <v>188673.921875</v>
       </c>
       <c r="R17" s="0">
         <v>9</v>
       </c>
       <c r="S17" s="0">
-        <v>448345.875</v>
+        <v>566021.75</v>
       </c>
       <c r="T17" s="0"/>
       <c r="U17" s="0"/>
       <c r="V17" s="0">
-        <v>597794.5</v>
+        <v>754695.6875</v>
       </c>
       <c r="W17" s="0">
         <v>2</v>
@@ -5814,13 +5814,13 @@
         <v>1</v>
       </c>
       <c r="AC17" s="0">
-        <v>597794.5</v>
+        <v>754695.6875</v>
       </c>
       <c r="AD17" s="0">
         <v>1</v>
       </c>
       <c r="AE17" s="0">
-        <v>597794.5</v>
+        <v>754695.6875</v>
       </c>
       <c r="AF17" s="0">
         <v>0</v>
@@ -5844,51 +5844,51 @@
         <v>1</v>
       </c>
       <c r="AM17" s="0">
-        <v>358676.71875</v>
+        <v>452817.4375</v>
       </c>
       <c r="AN17" s="0">
-        <v>89669.1796875</v>
+        <v>113204.359375</v>
       </c>
       <c r="AO17" s="0">
-        <v>119558.8984375</v>
+        <v>150939.140625</v>
       </c>
       <c r="AP17" s="0">
-        <v>29889.724609375</v>
+        <v>37734.78515625</v>
       </c>
       <c r="AQ17" s="0"/>
       <c r="AR17" s="0">
-        <v>478235.59375</v>
+        <v>603756.5625</v>
       </c>
       <c r="AS17" s="0"/>
       <c r="AT17" s="0"/>
       <c r="AU17" s="0"/>
       <c r="AV17" s="0">
-        <v>59779.44921875</v>
+        <v>75469.5703125</v>
       </c>
       <c r="AW17" s="0">
-        <v>59779.44921875</v>
+        <v>75469.5703125</v>
       </c>
       <c r="AX17" s="0">
-        <v>298897.25</v>
+        <v>377347.84375</v>
       </c>
       <c r="AY17" s="0">
-        <v>89669.1796875</v>
+        <v>113204.359375</v>
       </c>
       <c r="AZ17" s="0"/>
       <c r="BA17" s="0">
-        <v>59779.44921875</v>
+        <v>75469.5703125</v>
       </c>
       <c r="BB17" s="0"/>
       <c r="BC17" s="0">
-        <v>59779.44921875</v>
+        <v>75469.5703125</v>
       </c>
       <c r="BD17" s="0">
-        <v>59779.44921875</v>
+        <v>75469.5703125</v>
       </c>
       <c r="BE17" s="0"/>
       <c r="BF17" s="0"/>
       <c r="BG17" s="0">
-        <v>29889.724609375</v>
+        <v>37734.78515625</v>
       </c>
       <c r="BH17" s="0"/>
       <c r="BI17" s="0">
@@ -5968,7 +5968,7 @@
         <v>62</v>
       </c>
       <c r="CM17" s="0">
-        <v>597794.5625</v>
+        <v>754695.75</v>
       </c>
       <c r="CN17" s="0">
         <v>0</v>
@@ -5991,10 +5991,10 @@
         <v>58</v>
       </c>
       <c r="F18" s="0">
-        <v>534000</v>
+        <v>674157.3125</v>
       </c>
       <c r="G18" s="0">
-        <v>534000</v>
+        <v>674157.3125</v>
       </c>
       <c r="H18" s="0">
         <v>1</v>
@@ -6012,7 +6012,7 @@
         <v>14.010000228881836</v>
       </c>
       <c r="M18" s="0">
-        <v>38115.6328125</v>
+        <v>48119.72265625</v>
       </c>
       <c r="N18" s="0"/>
       <c r="O18" s="0"/>
@@ -6022,16 +6022,16 @@
         <v>3</v>
       </c>
       <c r="S18" s="0">
-        <v>114346.8984375</v>
+        <v>144359.171875</v>
       </c>
       <c r="T18" s="0">
         <v>11</v>
       </c>
       <c r="U18" s="0">
-        <v>419271.96875</v>
+        <v>529316.9375</v>
       </c>
       <c r="V18" s="0">
-        <v>533618.875</v>
+        <v>673676.125</v>
       </c>
       <c r="W18" s="0">
         <v>2</v>
@@ -6052,13 +6052,13 @@
         <v>1.0499999523162842</v>
       </c>
       <c r="AC18" s="0">
-        <v>560299.8125</v>
+        <v>707359.875</v>
       </c>
       <c r="AD18" s="0">
         <v>1</v>
       </c>
       <c r="AE18" s="0">
-        <v>560299.8125</v>
+        <v>707359.875</v>
       </c>
       <c r="AF18" s="0">
         <v>0</v>
@@ -6082,50 +6082,50 @@
         <v>1</v>
       </c>
       <c r="AM18" s="0">
-        <v>308164.90625</v>
+        <v>389047.9375</v>
       </c>
       <c r="AN18" s="0">
-        <v>112059.9609375</v>
+        <v>141471.984375</v>
       </c>
       <c r="AO18" s="0">
-        <v>56029.98046875</v>
+        <v>70735.9921875</v>
       </c>
       <c r="AP18" s="0">
-        <v>84044.9765625</v>
+        <v>106103.984375</v>
       </c>
       <c r="AQ18" s="0"/>
       <c r="AR18" s="0">
-        <v>448239.84375</v>
+        <v>565887.9375</v>
       </c>
       <c r="AS18" s="0"/>
       <c r="AT18" s="0"/>
       <c r="AU18" s="0"/>
       <c r="AV18" s="0">
-        <v>56029.98046875</v>
+        <v>70735.9921875</v>
       </c>
       <c r="AW18" s="0">
-        <v>56029.98046875</v>
+        <v>70735.9921875</v>
       </c>
       <c r="AX18" s="0">
-        <v>252134.90625</v>
+        <v>318311.9375</v>
       </c>
       <c r="AY18" s="0">
-        <v>56029.98046875</v>
+        <v>70735.9921875</v>
       </c>
       <c r="AZ18" s="0">
         <v>0</v>
       </c>
       <c r="BA18" s="0">
-        <v>84044.9765625</v>
+        <v>106103.984375</v>
       </c>
       <c r="BB18" s="0">
-        <v>28014.990234375</v>
+        <v>35367.99609375</v>
       </c>
       <c r="BC18" s="0">
-        <v>84044.9765625</v>
+        <v>106103.984375</v>
       </c>
       <c r="BD18" s="0">
-        <v>56029.98046875</v>
+        <v>70735.9921875</v>
       </c>
       <c r="BE18" s="0"/>
       <c r="BF18" s="0"/>
@@ -6210,7 +6210,7 @@
         <v>62</v>
       </c>
       <c r="CM18" s="0">
-        <v>560299.8125</v>
+        <v>707359.9375</v>
       </c>
       <c r="CN18" s="0">
         <v>0</v>
@@ -7485,7 +7485,7 @@
         <v>60</v>
       </c>
       <c r="F24" s="0">
-        <v>182895</v>
+        <v>230898.875</v>
       </c>
       <c r="G24" s="0">
         <v>20.628416061401367</v>
@@ -9075,13 +9075,13 @@
         <v>60</v>
       </c>
       <c r="F31" s="0">
-        <v>2309270.5</v>
+        <v>2915377.5</v>
       </c>
       <c r="G31" s="0">
         <v>825354.125</v>
       </c>
       <c r="H31" s="0">
-        <v>0.36000001430511475</v>
+        <v>0.2800000011920929</v>
       </c>
       <c r="I31" s="1">
         <v>43586</v>
@@ -9267,13 +9267,13 @@
         <v>60</v>
       </c>
       <c r="F32" s="0">
-        <v>4361000</v>
+        <v>5505618</v>
       </c>
       <c r="G32" s="0">
         <v>4043587</v>
       </c>
       <c r="H32" s="0">
-        <v>0.93000000715255737</v>
+        <v>0.73000001907348633</v>
       </c>
       <c r="I32" s="1">
         <v>42552</v>
@@ -9673,7 +9673,7 @@
         <v>58</v>
       </c>
       <c r="F34" s="0">
-        <v>89000</v>
+        <v>112359.546875</v>
       </c>
       <c r="G34" s="0">
         <v>0</v>
@@ -9935,10 +9935,10 @@
         <v>58</v>
       </c>
       <c r="F35" s="0">
-        <v>267000</v>
+        <v>337078.65625</v>
       </c>
       <c r="G35" s="0">
-        <v>70191.6328125</v>
+        <v>88614.609375</v>
       </c>
       <c r="H35" s="0">
         <v>0.25999999046325684</v>
@@ -9956,7 +9956,7 @@
         <v>24</v>
       </c>
       <c r="M35" s="0">
-        <v>2924.6513671875</v>
+        <v>3692.275390625</v>
       </c>
       <c r="N35" s="0"/>
       <c r="O35" s="0"/>
@@ -9968,10 +9968,10 @@
         <v>6</v>
       </c>
       <c r="U35" s="0">
-        <v>17547.908203125</v>
+        <v>22153.65234375</v>
       </c>
       <c r="V35" s="0">
-        <v>17547.908203125</v>
+        <v>22153.65234375</v>
       </c>
       <c r="W35" s="0">
         <v>3</v>
@@ -9992,13 +9992,13 @@
         <v>0.5</v>
       </c>
       <c r="AC35" s="0">
-        <v>8773.9541015625</v>
+        <v>11076.826171875</v>
       </c>
       <c r="AD35" s="0">
         <v>1</v>
       </c>
       <c r="AE35" s="0">
-        <v>8773.9501953125</v>
+        <v>11076.830078125</v>
       </c>
       <c r="AF35" s="0">
         <v>0</v>
@@ -10022,7 +10022,7 @@
         <v>1</v>
       </c>
       <c r="AM35" s="0">
-        <v>8773.9501953125</v>
+        <v>11076.830078125</v>
       </c>
       <c r="AN35" s="0">
         <v>0</v>
@@ -10037,7 +10037,7 @@
         <v>0</v>
       </c>
       <c r="AR35" s="0">
-        <v>8773.9501953125</v>
+        <v>11076.830078125</v>
       </c>
       <c r="AS35" s="0">
         <v>0</v>
@@ -10055,7 +10055,7 @@
         <v>0</v>
       </c>
       <c r="AX35" s="0">
-        <v>8773.9501953125</v>
+        <v>11076.830078125</v>
       </c>
       <c r="AY35" s="0">
         <v>0</v>
@@ -10174,7 +10174,7 @@
         <v>62</v>
       </c>
       <c r="CM35" s="0">
-        <v>8773.9501953125</v>
+        <v>11076.830078125</v>
       </c>
       <c r="CN35" s="0">
         <v>0</v>
@@ -10197,10 +10197,10 @@
         <v>58</v>
       </c>
       <c r="F36" s="0">
-        <v>123860.40625</v>
+        <v>156369.65625</v>
       </c>
       <c r="G36" s="0">
-        <v>117455.078125</v>
+        <v>148283.140625</v>
       </c>
       <c r="H36" s="0">
         <v>0.94999998807907104</v>
@@ -10218,26 +10218,26 @@
         <v>11.970000267028809</v>
       </c>
       <c r="M36" s="0">
-        <v>9812.4541015625</v>
+        <v>12387.8974609375</v>
       </c>
       <c r="N36" s="0">
         <v>2.9000000953674316</v>
       </c>
       <c r="O36" s="0">
-        <v>28456.1171875</v>
+        <v>35924.90234375</v>
       </c>
       <c r="P36" s="0">
         <v>9</v>
       </c>
       <c r="Q36" s="0">
-        <v>88312.0859375</v>
+        <v>111491.078125</v>
       </c>
       <c r="R36" s="0"/>
       <c r="S36" s="0"/>
       <c r="T36" s="0"/>
       <c r="U36" s="0"/>
       <c r="V36" s="0">
-        <v>88312.0859375</v>
+        <v>35924.90234375</v>
       </c>
       <c r="W36" s="0">
         <v>2</v>
@@ -10258,19 +10258,19 @@
         <v>1</v>
       </c>
       <c r="AC36" s="0">
-        <v>88312.0859375</v>
+        <v>35924.90234375</v>
       </c>
       <c r="AD36" s="0">
         <v>1</v>
       </c>
       <c r="AE36" s="0">
-        <v>88312.09375</v>
+        <v>35924.8984375</v>
       </c>
       <c r="AF36" s="0">
         <v>0.56000000238418579</v>
       </c>
       <c r="AG36" s="0">
-        <v>49454.76953125</v>
+        <v>20117.9453125</v>
       </c>
       <c r="AH36" s="0">
         <v>0.49000000953674316</v>
@@ -10288,22 +10288,22 @@
         <v>1</v>
       </c>
       <c r="AM36" s="0">
-        <v>43272.92578125</v>
+        <v>17603.201171875</v>
       </c>
       <c r="AN36" s="0">
-        <v>19428.66015625</v>
+        <v>7903.4775390625</v>
       </c>
       <c r="AO36" s="0">
         <v>0</v>
       </c>
       <c r="AP36" s="0">
-        <v>25610.505859375</v>
+        <v>10418.220703125</v>
       </c>
       <c r="AQ36" s="0">
         <v>0</v>
       </c>
       <c r="AR36" s="0">
-        <v>88312.09375</v>
+        <v>35924.8984375</v>
       </c>
       <c r="AS36" s="0">
         <v>0</v>
@@ -10324,15 +10324,15 @@
         <v>0</v>
       </c>
       <c r="AY36" s="0">
-        <v>15896.177734375</v>
+        <v>6466.48193359375</v>
       </c>
       <c r="AZ36" s="0"/>
       <c r="BA36" s="0"/>
       <c r="BB36" s="0">
-        <v>10597.451171875</v>
+        <v>4310.98779296875</v>
       </c>
       <c r="BC36" s="0">
-        <v>12363.693359375</v>
+        <v>5029.48583984375</v>
       </c>
       <c r="BD36" s="0"/>
       <c r="BE36" s="0"/>
@@ -10420,7 +10420,7 @@
         <v>489</v>
       </c>
       <c r="CM36" s="0">
-        <v>88312.09375</v>
+        <v>35924.8984375</v>
       </c>
       <c r="CN36" s="0">
         <v>0</v>
@@ -10943,10 +10943,10 @@
         <v>58</v>
       </c>
       <c r="F39" s="0">
-        <v>890000</v>
+        <v>1123595.5</v>
       </c>
       <c r="G39" s="0">
-        <v>44500</v>
+        <v>56179.7734375</v>
       </c>
       <c r="H39" s="0">
         <v>0.05000000074505806</v>
@@ -10964,7 +10964,7 @@
         <v>2.9600000381469727</v>
       </c>
       <c r="M39" s="0">
-        <v>15033.783203125</v>
+        <v>18979.65234375</v>
       </c>
       <c r="N39" s="0"/>
       <c r="O39" s="0"/>
@@ -10976,10 +10976,10 @@
         <v>3</v>
       </c>
       <c r="U39" s="0">
-        <v>45101.3515625</v>
+        <v>56938.95703125</v>
       </c>
       <c r="V39" s="0">
-        <v>45101.3515625</v>
+        <v>56938.95703125</v>
       </c>
       <c r="W39" s="0">
         <v>3</v>
@@ -11000,13 +11000,13 @@
         <v>1.0499999523162842</v>
       </c>
       <c r="AC39" s="0">
-        <v>47356.41796875</v>
+        <v>59785.90234375</v>
       </c>
       <c r="AD39" s="0">
         <v>1</v>
       </c>
       <c r="AE39" s="0">
-        <v>47356.421875</v>
+        <v>59785.8984375</v>
       </c>
       <c r="AF39" s="0">
         <v>0</v>
@@ -11030,22 +11030,22 @@
         <v>1</v>
       </c>
       <c r="AM39" s="0">
-        <v>30781.673828125</v>
+        <v>38860.83203125</v>
       </c>
       <c r="AN39" s="0">
-        <v>11839.10546875</v>
+        <v>14946.474609375</v>
       </c>
       <c r="AO39" s="0">
-        <v>2367.821044921875</v>
+        <v>2989.294921875</v>
       </c>
       <c r="AP39" s="0">
-        <v>2367.821044921875</v>
+        <v>2989.294921875</v>
       </c>
       <c r="AQ39" s="0">
         <v>0</v>
       </c>
       <c r="AR39" s="0">
-        <v>37885.13671875</v>
+        <v>47828.71875</v>
       </c>
       <c r="AS39" s="0">
         <v>0</v>
@@ -11054,40 +11054,40 @@
         <v>0</v>
       </c>
       <c r="AU39" s="0">
-        <v>4735.64208984375</v>
+        <v>5978.58984375</v>
       </c>
       <c r="AV39" s="0">
-        <v>2367.821044921875</v>
+        <v>2989.294921875</v>
       </c>
       <c r="AW39" s="0">
-        <v>2367.821044921875</v>
+        <v>2989.294921875</v>
       </c>
       <c r="AX39" s="0">
-        <v>11839.10546875</v>
+        <v>14946.474609375</v>
       </c>
       <c r="AY39" s="0">
-        <v>7103.46337890625</v>
+        <v>8967.884765625</v>
       </c>
       <c r="AZ39" s="0">
-        <v>2367.821044921875</v>
+        <v>2989.294921875</v>
       </c>
       <c r="BA39" s="0">
-        <v>7103.46337890625</v>
+        <v>8967.884765625</v>
       </c>
       <c r="BB39" s="0">
-        <v>7103.46337890625</v>
+        <v>8967.884765625</v>
       </c>
       <c r="BC39" s="0">
-        <v>4735.64208984375</v>
+        <v>5978.58984375</v>
       </c>
       <c r="BD39" s="0">
-        <v>4735.64208984375</v>
+        <v>5978.58984375</v>
       </c>
       <c r="BE39" s="0">
         <v>0</v>
       </c>
       <c r="BF39" s="0">
-        <v>2367.821044921875</v>
+        <v>2989.294921875</v>
       </c>
       <c r="BG39" s="0">
         <v>0</v>
@@ -11186,7 +11186,7 @@
         <v>62</v>
       </c>
       <c r="CM39" s="0">
-        <v>47356.421875</v>
+        <v>59785.8984375</v>
       </c>
       <c r="CN39" s="0">
         <v>0</v>
@@ -11479,10 +11479,10 @@
         <v>58</v>
       </c>
       <c r="F41" s="0">
-        <v>13404399</v>
+        <v>16922608</v>
       </c>
       <c r="G41" s="0">
-        <v>7253267.5</v>
+        <v>9157010</v>
       </c>
       <c r="H41" s="0">
         <v>0.54000002145767212</v>
@@ -11500,34 +11500,34 @@
         <v>29.950000762939453</v>
       </c>
       <c r="M41" s="0">
-        <v>242179.203125</v>
+        <v>305743.21875</v>
       </c>
       <c r="N41" s="0">
         <v>4.9000000953674316</v>
       </c>
       <c r="O41" s="0">
-        <v>1186678.125</v>
+        <v>1498141.75</v>
       </c>
       <c r="P41" s="0">
         <v>4.9000000953674316</v>
       </c>
       <c r="Q41" s="0">
-        <v>1186678.125</v>
+        <v>1498141.75</v>
       </c>
       <c r="R41" s="0">
         <v>12</v>
       </c>
       <c r="S41" s="0">
-        <v>2906150.5</v>
+        <v>3668918.5</v>
       </c>
       <c r="T41" s="0">
         <v>12</v>
       </c>
       <c r="U41" s="0">
-        <v>2906150.5</v>
+        <v>3668918.5</v>
       </c>
       <c r="V41" s="0">
-        <v>6998979</v>
+        <v>8835978</v>
       </c>
       <c r="W41" s="0">
         <v>6</v>
@@ -11548,13 +11548,13 @@
         <v>1.0099999904632568</v>
       </c>
       <c r="AC41" s="0">
-        <v>7068968.5</v>
+        <v>8924338</v>
       </c>
       <c r="AD41" s="0">
         <v>1</v>
       </c>
       <c r="AE41" s="0">
-        <v>7068968.5</v>
+        <v>8924338</v>
       </c>
       <c r="AF41" s="0">
         <v>0</v>
@@ -11578,13 +11578,13 @@
         <v>1</v>
       </c>
       <c r="AM41" s="0">
-        <v>2403449.25</v>
+        <v>3034275</v>
       </c>
       <c r="AN41" s="0">
-        <v>4594829.5</v>
+        <v>5800819.5</v>
       </c>
       <c r="AO41" s="0">
-        <v>70689.6796875</v>
+        <v>89243.375</v>
       </c>
       <c r="AP41" s="0">
         <v>0</v>
@@ -11593,46 +11593,46 @@
         <v>0</v>
       </c>
       <c r="AR41" s="0">
-        <v>4948278</v>
+        <v>6247036.5</v>
       </c>
       <c r="AS41" s="0">
         <v>0</v>
       </c>
       <c r="AT41" s="0">
-        <v>2050000.75</v>
+        <v>2588058</v>
       </c>
       <c r="AU41" s="0">
         <v>0</v>
       </c>
       <c r="AV41" s="0">
-        <v>70689.6796875</v>
+        <v>89243.375</v>
       </c>
       <c r="AW41" s="0">
         <v>0</v>
       </c>
       <c r="AX41" s="0">
-        <v>2403449.25</v>
+        <v>3034275</v>
       </c>
       <c r="AY41" s="0">
-        <v>1413793.75</v>
+        <v>1784867.625</v>
       </c>
       <c r="AZ41" s="0">
-        <v>848276.1875</v>
+        <v>1070920.5</v>
       </c>
       <c r="BA41" s="0">
-        <v>848276.1875</v>
+        <v>1070920.5</v>
       </c>
       <c r="BB41" s="0">
-        <v>353448.4375</v>
+        <v>446216.90625</v>
       </c>
       <c r="BC41" s="0">
-        <v>1060345.375</v>
+        <v>1338650.75</v>
       </c>
       <c r="BD41" s="0">
-        <v>70689.6796875</v>
+        <v>89243.375</v>
       </c>
       <c r="BE41" s="0">
-        <v>70689.6796875</v>
+        <v>89243.375</v>
       </c>
       <c r="BF41" s="0">
         <v>0</v>
@@ -11734,10 +11734,10 @@
         <v>461</v>
       </c>
       <c r="CM41" s="0">
-        <v>7068968.5</v>
+        <v>8924337</v>
       </c>
       <c r="CN41" s="0">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="42">
@@ -11757,10 +11757,10 @@
         <v>58</v>
       </c>
       <c r="F42" s="0">
-        <v>2704842.5</v>
+        <v>3414774.25</v>
       </c>
       <c r="G42" s="0">
-        <v>2686485.5</v>
+        <v>3391599</v>
       </c>
       <c r="H42" s="0">
         <v>0.99000000953674316</v>
@@ -11778,34 +11778,34 @@
         <v>47.049999237060547</v>
       </c>
       <c r="M42" s="0">
-        <v>57098.5234375</v>
+        <v>72084.9921875</v>
       </c>
       <c r="N42" s="0">
         <v>12</v>
       </c>
       <c r="O42" s="0">
-        <v>685182.25</v>
+        <v>865019.875</v>
       </c>
       <c r="P42" s="0">
         <v>12</v>
       </c>
       <c r="Q42" s="0">
-        <v>685182.25</v>
+        <v>865019.875</v>
       </c>
       <c r="R42" s="0">
         <v>12</v>
       </c>
       <c r="S42" s="0">
-        <v>685182.25</v>
+        <v>865019.875</v>
       </c>
       <c r="T42" s="0">
         <v>12</v>
       </c>
       <c r="U42" s="0">
-        <v>685182.25</v>
+        <v>865019.875</v>
       </c>
       <c r="V42" s="0">
-        <v>2055546.75</v>
+        <v>2595059.5</v>
       </c>
       <c r="W42" s="0">
         <v>4</v>
@@ -11826,19 +11826,19 @@
         <v>1.0199999809265137</v>
       </c>
       <c r="AC42" s="0">
-        <v>2096657.625</v>
+        <v>2646960.75</v>
       </c>
       <c r="AD42" s="0">
         <v>0.60000002384185791</v>
       </c>
       <c r="AE42" s="0">
-        <v>1257994.625</v>
+        <v>1588176.5</v>
       </c>
       <c r="AF42" s="0">
         <v>0.40000000596046448</v>
       </c>
       <c r="AG42" s="0">
-        <v>838663.0625</v>
+        <v>1058784.375</v>
       </c>
       <c r="AH42" s="0">
         <v>0.25</v>
@@ -11856,13 +11856,13 @@
         <v>1</v>
       </c>
       <c r="AM42" s="0">
-        <v>314498.65625</v>
+        <v>397044.125</v>
       </c>
       <c r="AN42" s="0">
-        <v>805116.5625</v>
+        <v>1016432.9375</v>
       </c>
       <c r="AO42" s="0">
-        <v>138379.40625</v>
+        <v>174699.40625</v>
       </c>
       <c r="AP42" s="0">
         <v>0</v>
@@ -11877,40 +11877,40 @@
         <v>0</v>
       </c>
       <c r="AT42" s="0">
-        <v>1119615.25</v>
+        <v>1413477</v>
       </c>
       <c r="AU42" s="0">
         <v>0</v>
       </c>
       <c r="AV42" s="0">
-        <v>138379.40625</v>
+        <v>174699.40625</v>
       </c>
       <c r="AW42" s="0">
         <v>0</v>
       </c>
       <c r="AX42" s="0">
-        <v>314498.65625</v>
+        <v>397044.125</v>
       </c>
       <c r="AY42" s="0">
-        <v>100639.5703125</v>
+        <v>127054.1171875</v>
       </c>
       <c r="AZ42" s="0">
-        <v>427718.1875</v>
+        <v>539980</v>
       </c>
       <c r="BA42" s="0">
-        <v>150959.359375</v>
+        <v>190581.171875</v>
       </c>
       <c r="BB42" s="0">
-        <v>113219.5234375</v>
+        <v>142935.890625</v>
       </c>
       <c r="BC42" s="0">
-        <v>88059.625</v>
+        <v>111172.359375</v>
       </c>
       <c r="BD42" s="0">
-        <v>37739.83984375</v>
+        <v>47645.29296875</v>
       </c>
       <c r="BE42" s="0">
-        <v>25159.892578125</v>
+        <v>31763.529296875</v>
       </c>
       <c r="BF42" s="0">
         <v>0</v>
@@ -12012,7 +12012,7 @@
         <v>491</v>
       </c>
       <c r="CM42" s="0">
-        <v>1257994.625</v>
+        <v>1588176.375</v>
       </c>
       <c r="CN42" s="0">
         <v>0</v>
@@ -12035,10 +12035,10 @@
         <v>58</v>
       </c>
       <c r="F43" s="0">
-        <v>3491412.25</v>
+        <v>4407792</v>
       </c>
       <c r="G43" s="0">
-        <v>1992182.25</v>
+        <v>2515064</v>
       </c>
       <c r="H43" s="0">
         <v>0.56999999284744263</v>
@@ -12056,34 +12056,34 @@
         <v>31.989999771118164</v>
       </c>
       <c r="M43" s="0">
-        <v>62275.15625</v>
+        <v>78620.3203125</v>
       </c>
       <c r="N43" s="0">
         <v>6.9000000953674316</v>
       </c>
       <c r="O43" s="0">
-        <v>429698.59375</v>
+        <v>542480.1875</v>
       </c>
       <c r="P43" s="0">
         <v>6.9000000953674316</v>
       </c>
       <c r="Q43" s="0">
-        <v>429698.59375</v>
+        <v>542480.1875</v>
       </c>
       <c r="R43" s="0">
         <v>12</v>
       </c>
       <c r="S43" s="0">
-        <v>747301.875</v>
+        <v>943443.875</v>
       </c>
       <c r="T43" s="0">
         <v>12</v>
       </c>
       <c r="U43" s="0">
-        <v>747301.875</v>
+        <v>943443.875</v>
       </c>
       <c r="V43" s="0">
-        <v>1924302.375</v>
+        <v>2429368</v>
       </c>
       <c r="W43" s="0">
         <v>1</v>
@@ -12104,13 +12104,13 @@
         <v>1</v>
       </c>
       <c r="AC43" s="0">
-        <v>1924302.375</v>
+        <v>2429368</v>
       </c>
       <c r="AD43" s="0">
         <v>1</v>
       </c>
       <c r="AE43" s="0">
-        <v>1924302.375</v>
+        <v>2429368</v>
       </c>
       <c r="AF43" s="0">
         <v>0</v>
@@ -12134,59 +12134,59 @@
         <v>1</v>
       </c>
       <c r="AM43" s="0">
-        <v>1347011.625</v>
+        <v>1700557.625</v>
       </c>
       <c r="AN43" s="0">
-        <v>481075.59375</v>
+        <v>607342</v>
       </c>
       <c r="AO43" s="0">
-        <v>96215.1171875</v>
+        <v>121468.3984375</v>
       </c>
       <c r="AP43" s="0">
         <v>0</v>
       </c>
       <c r="AQ43" s="0"/>
       <c r="AR43" s="0">
-        <v>1539441.875</v>
+        <v>1943494.375</v>
       </c>
       <c r="AS43" s="0"/>
       <c r="AT43" s="0">
-        <v>288645.375</v>
+        <v>364405.21875</v>
       </c>
       <c r="AU43" s="0">
         <v>0</v>
       </c>
       <c r="AV43" s="0">
-        <v>96215.1171875</v>
+        <v>121468.3984375</v>
       </c>
       <c r="AW43" s="0"/>
       <c r="AX43" s="0">
-        <v>1347011.625</v>
+        <v>1700557.625</v>
       </c>
       <c r="AY43" s="0">
-        <v>250159.296875</v>
+        <v>315817.84375</v>
       </c>
       <c r="AZ43" s="0">
-        <v>76972.09375</v>
+        <v>97174.71875</v>
       </c>
       <c r="BA43" s="0">
-        <v>76972.09375</v>
+        <v>97174.71875</v>
       </c>
       <c r="BB43" s="0">
-        <v>38486.046875</v>
+        <v>48587.359375</v>
       </c>
       <c r="BC43" s="0">
-        <v>96215.1171875</v>
+        <v>121468.3984375</v>
       </c>
       <c r="BD43" s="0">
-        <v>19243.0234375</v>
+        <v>24293.6796875</v>
       </c>
       <c r="BE43" s="0">
         <v>0</v>
       </c>
       <c r="BF43" s="0"/>
       <c r="BG43" s="0">
-        <v>19243.0234375</v>
+        <v>24293.6796875</v>
       </c>
       <c r="BH43" s="0"/>
       <c r="BI43" s="0">
@@ -12274,7 +12274,7 @@
         <v>461</v>
       </c>
       <c r="CM43" s="0">
-        <v>1924302.375</v>
+        <v>2429368</v>
       </c>
       <c r="CN43" s="0">
         <v>0</v>
@@ -13083,13 +13083,13 @@
         <v>60</v>
       </c>
       <c r="F47" s="0">
-        <v>22740000</v>
+        <v>39577836</v>
       </c>
       <c r="G47" s="0">
         <v>16693989</v>
       </c>
       <c r="H47" s="0">
-        <v>0.73000001907348633</v>
+        <v>0.41999998688697815</v>
       </c>
       <c r="I47" s="1">
         <v>43101</v>
@@ -13737,7 +13737,7 @@
         <v>60</v>
       </c>
       <c r="F50" s="0">
-        <v>2987798.5</v>
+        <v>3771996.75</v>
       </c>
       <c r="G50" s="0">
         <v>576.9552001953125</v>
@@ -14415,13 +14415,13 @@
         <v>60</v>
       </c>
       <c r="F53" s="0">
-        <v>54129.80078125</v>
+        <v>68337.078125</v>
       </c>
       <c r="G53" s="0">
         <v>69636.2421875</v>
       </c>
       <c r="H53" s="0">
-        <v>1.2899999618530273</v>
+        <v>1.0199999809265137</v>
       </c>
       <c r="I53" s="1">
         <v>43101</v>
@@ -15055,13 +15055,13 @@
         <v>60</v>
       </c>
       <c r="F56" s="0">
-        <v>115700</v>
+        <v>146067.421875</v>
       </c>
       <c r="G56" s="0">
         <v>69523.9375</v>
       </c>
       <c r="H56" s="0">
-        <v>0.60000002384185791</v>
+        <v>0.47999998927116394</v>
       </c>
       <c r="I56" s="1">
         <v>43739</v>
@@ -15467,13 +15467,13 @@
         <v>60</v>
       </c>
       <c r="F58" s="0">
-        <v>89000</v>
+        <v>112359.546875</v>
       </c>
       <c r="G58" s="0">
         <v>114495.625</v>
       </c>
       <c r="H58" s="0">
-        <v>1.2899999618530273</v>
+        <v>1.0199999809265137</v>
       </c>
       <c r="I58" s="1">
         <v>43101</v>
@@ -15507,7 +15507,7 @@
       <c r="T58" s="0"/>
       <c r="U58" s="0"/>
       <c r="V58" s="0">
-        <v>809565.0625</v>
+        <v>115652.1484375</v>
       </c>
       <c r="W58" s="0">
         <v>1</v>
@@ -15526,13 +15526,13 @@
         <v>1</v>
       </c>
       <c r="AC58" s="0">
-        <v>809565.0625</v>
+        <v>115652.1484375</v>
       </c>
       <c r="AD58" s="0">
         <v>1</v>
       </c>
       <c r="AE58" s="0">
-        <v>809565.0625</v>
+        <v>115652.1484375</v>
       </c>
       <c r="AF58" s="0">
         <v>0</v>
@@ -15550,7 +15550,7 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="AM58" s="0">
-        <v>728608.5625</v>
+        <v>104086.9296875</v>
       </c>
       <c r="AN58" s="0"/>
       <c r="AO58" s="0"/>
@@ -15558,7 +15558,7 @@
       <c r="AQ58" s="0"/>
       <c r="AR58" s="0"/>
       <c r="AS58" s="0">
-        <v>809565.0625</v>
+        <v>115652.1484375</v>
       </c>
       <c r="AT58" s="0"/>
       <c r="AU58" s="0"/>
@@ -15569,7 +15569,7 @@
       <c r="AZ58" s="0"/>
       <c r="BA58" s="0"/>
       <c r="BB58" s="0">
-        <v>809565.0625</v>
+        <v>115652.1484375</v>
       </c>
       <c r="BC58" s="0"/>
       <c r="BD58" s="0"/>
@@ -15640,10 +15640,10 @@
         <v>62</v>
       </c>
       <c r="CM58" s="0">
-        <v>728608.5625</v>
+        <v>104086.9296875</v>
       </c>
       <c r="CN58" s="0">
-        <v>-80956</v>
+        <v>-11565</v>
       </c>
     </row>
     <row r="59">
@@ -15923,7 +15923,7 @@
       <c r="T60" s="0"/>
       <c r="U60" s="0"/>
       <c r="V60" s="0">
-        <v>3194941.5</v>
+        <v>456420.21875</v>
       </c>
       <c r="W60" s="0">
         <v>1</v>
@@ -15942,13 +15942,13 @@
         <v>1</v>
       </c>
       <c r="AC60" s="0">
-        <v>3194941.5</v>
+        <v>456420.21875</v>
       </c>
       <c r="AD60" s="0">
         <v>1</v>
       </c>
       <c r="AE60" s="0">
-        <v>3194941.5</v>
+        <v>456420.21875</v>
       </c>
       <c r="AF60" s="0">
         <v>0</v>
@@ -15968,39 +15968,39 @@
         <v>1</v>
       </c>
       <c r="AM60" s="0">
-        <v>2236459</v>
+        <v>319494.15625</v>
       </c>
       <c r="AN60" s="0">
-        <v>958482.5</v>
+        <v>136926.078125</v>
       </c>
       <c r="AO60" s="0"/>
       <c r="AP60" s="0"/>
       <c r="AQ60" s="0"/>
       <c r="AR60" s="0"/>
       <c r="AS60" s="0">
-        <v>3194941.5</v>
+        <v>456420.21875</v>
       </c>
       <c r="AT60" s="0"/>
       <c r="AU60" s="0"/>
       <c r="AV60" s="0"/>
       <c r="AW60" s="0"/>
       <c r="AX60" s="0">
-        <v>287544.75</v>
+        <v>41077.8203125</v>
       </c>
       <c r="AY60" s="0">
-        <v>383392.96875</v>
+        <v>54770.42578125</v>
       </c>
       <c r="AZ60" s="0">
-        <v>1150179</v>
+        <v>164311.28125</v>
       </c>
       <c r="BA60" s="0">
-        <v>159747.078125</v>
+        <v>22821.01171875</v>
       </c>
       <c r="BB60" s="0">
-        <v>1054330.75</v>
+        <v>150618.671875</v>
       </c>
       <c r="BC60" s="0">
-        <v>159747.078125</v>
+        <v>22821.01171875</v>
       </c>
       <c r="BD60" s="0"/>
       <c r="BE60" s="0"/>
@@ -16080,7 +16080,7 @@
         <v>62</v>
       </c>
       <c r="CM60" s="0">
-        <v>3194941.5</v>
+        <v>456420.25</v>
       </c>
       <c r="CN60" s="0">
         <v>0</v>
@@ -16317,10 +16317,10 @@
         <v>58</v>
       </c>
       <c r="F62" s="0">
-        <v>25810000</v>
+        <v>32584270</v>
       </c>
       <c r="G62" s="0">
-        <v>20915000</v>
+        <v>26404494</v>
       </c>
       <c r="H62" s="0">
         <v>0.81000000238418579</v>
@@ -16338,34 +16338,34 @@
         <v>48</v>
       </c>
       <c r="M62" s="0">
-        <v>435729.15625</v>
+        <v>550093.625</v>
       </c>
       <c r="N62" s="0">
         <v>12</v>
       </c>
       <c r="O62" s="0">
-        <v>5228750</v>
+        <v>6601123.5</v>
       </c>
       <c r="P62" s="0">
         <v>12</v>
       </c>
       <c r="Q62" s="0">
-        <v>5228750</v>
+        <v>6601123.5</v>
       </c>
       <c r="R62" s="0">
         <v>12</v>
       </c>
       <c r="S62" s="0">
-        <v>5228750</v>
+        <v>6601123.5</v>
       </c>
       <c r="T62" s="0">
         <v>12</v>
       </c>
       <c r="U62" s="0">
-        <v>5228750</v>
+        <v>6601123.5</v>
       </c>
       <c r="V62" s="0">
-        <v>15686250</v>
+        <v>19803370</v>
       </c>
       <c r="W62" s="0">
         <v>6</v>
@@ -16386,13 +16386,13 @@
         <v>0.5</v>
       </c>
       <c r="AC62" s="0">
-        <v>7843125</v>
+        <v>9901685</v>
       </c>
       <c r="AD62" s="0">
         <v>0.25</v>
       </c>
       <c r="AE62" s="0">
-        <v>1960781.25</v>
+        <v>2475421.25</v>
       </c>
       <c r="AF62" s="0">
         <v>0</v>
@@ -16414,13 +16414,13 @@
         <v>1</v>
       </c>
       <c r="AM62" s="0">
-        <v>784312.5</v>
+        <v>990168.5</v>
       </c>
       <c r="AN62" s="0">
-        <v>980390.625</v>
+        <v>1237710.625</v>
       </c>
       <c r="AO62" s="0">
-        <v>196078.125</v>
+        <v>247542.125</v>
       </c>
       <c r="AP62" s="0"/>
       <c r="AQ62" s="0"/>
@@ -16428,7 +16428,7 @@
       <c r="AS62" s="0"/>
       <c r="AT62" s="0"/>
       <c r="AU62" s="0">
-        <v>1960781.25</v>
+        <v>2475421.25</v>
       </c>
       <c r="AV62" s="0"/>
       <c r="AW62" s="0"/>
@@ -16437,11 +16437,11 @@
       <c r="AZ62" s="0"/>
       <c r="BA62" s="0"/>
       <c r="BB62" s="0">
-        <v>1764703.125</v>
+        <v>2227879</v>
       </c>
       <c r="BC62" s="0"/>
       <c r="BD62" s="0">
-        <v>196078.125</v>
+        <v>247542.125</v>
       </c>
       <c r="BE62" s="0"/>
       <c r="BF62" s="0"/>
@@ -16512,7 +16512,7 @@
         <v>62</v>
       </c>
       <c r="CM62" s="0">
-        <v>1960781.25</v>
+        <v>2475421</v>
       </c>
       <c r="CN62" s="0">
         <v>0</v>

</xml_diff>

<commit_message>
table for power bi created
</commit_message>
<xml_diff>
--- a/clean_data/ERP_projects.xlsx
+++ b/clean_data/ERP_projects.xlsx
@@ -1342,19 +1342,19 @@
         <v>220</v>
       </c>
       <c r="CS2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="CT2" t="s">
         <v>221</v>
       </c>
       <c r="CU2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="CV2" t="s">
         <v>221</v>
       </c>
       <c r="CW2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="CX2" t="s">
         <v>232</v>
@@ -6215,10 +6215,10 @@
         <v>1</v>
       </c>
       <c r="CP21" t="s">
+        <v>222</v>
+      </c>
+      <c r="CQ21" t="s">
         <v>221</v>
-      </c>
-      <c r="CQ21" t="s">
-        <v>222</v>
       </c>
       <c r="CR21" t="s">
         <v>128</v>
@@ -16345,10 +16345,10 @@
         <v>1.0000001192092896</v>
       </c>
       <c r="CP58" t="s">
+        <v>221</v>
+      </c>
+      <c r="CQ58" t="s">
         <v>222</v>
-      </c>
-      <c r="CQ58" t="s">
-        <v>221</v>
       </c>
       <c r="CR58" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
clean project table for dashboard
</commit_message>
<xml_diff>
--- a/clean_data/ERP_projects.xlsx
+++ b/clean_data/ERP_projects.xlsx
@@ -1342,19 +1342,19 @@
         <v>220</v>
       </c>
       <c r="CS2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="CT2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="CU2" t="s">
         <v>221</v>
       </c>
       <c r="CV2" t="s">
+        <v>222</v>
+      </c>
+      <c r="CW2" t="s">
         <v>221</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>220</v>
       </c>
       <c r="CX2" t="s">
         <v>232</v>
@@ -6215,10 +6215,10 @@
         <v>1</v>
       </c>
       <c r="CP21" t="s">
+        <v>221</v>
+      </c>
+      <c r="CQ21" t="s">
         <v>222</v>
-      </c>
-      <c r="CQ21" t="s">
-        <v>221</v>
       </c>
       <c r="CR21" t="s">
         <v>128</v>
@@ -13081,10 +13081,10 @@
         <v>1</v>
       </c>
       <c r="CP46" t="s">
+        <v>222</v>
+      </c>
+      <c r="CQ46" t="s">
         <v>221</v>
-      </c>
-      <c r="CQ46" t="s">
-        <v>222</v>
       </c>
       <c r="CR46" t="s">
         <v>222</v>

</xml_diff>

<commit_message>
joint version of the data for dashboard
</commit_message>
<xml_diff>
--- a/clean_data/ERP_projects.xlsx
+++ b/clean_data/ERP_projects.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2105" uniqueCount="314">
   <si>
     <t>ID</t>
   </si>
@@ -772,6 +772,189 @@
   </si>
   <si>
     <t>implementor_summary</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000036009&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000036019&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000036033&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000036043&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000036053&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000036063&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000036073&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000036083&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000036093&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000036103&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000037009&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000037019&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000037025&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000038025&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000039009&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000039023&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000040153&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000040163&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000041009&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000041039&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000042073&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000043013&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000043019&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000044021&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000044035&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000044045&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000044055&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000044073&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000045097&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000045175&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000045197&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000046009&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000046019&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000046029&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000046049&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000048013&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000049011&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000050013&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000050023&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000050037&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000050055&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000050065&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000050075&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000050085&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000050099&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000050121&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000051009&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000051023&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000051037&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000051051&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000051085&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000052009&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000054045&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000055053&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000056021&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000057017&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000058021&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000059029&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000061069&amp;viewLinkName=Project_spending</t>
+  </si>
+  <si>
+    <t>https://app.zohocreator.eu/erp.forms20/erp/#Form:Projects?recLinkID=88734000000063017&amp;viewLinkName=Project_spending</t>
   </si>
 </sst>
 </file>
@@ -817,7 +1000,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DT61"/>
+  <dimension ref="A1:DU61"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -1192,6 +1375,9 @@
       </c>
       <c r="DT1" t="s">
         <v>252</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="2">
@@ -1503,6 +1689,9 @@
       <c r="DT2" t="s">
         <v>120</v>
       </c>
+      <c r="DU2" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -1820,6 +2009,9 @@
       </c>
       <c r="DT3" t="s">
         <v>120</v>
+      </c>
+      <c r="DU3" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="4">
@@ -2111,6 +2303,9 @@
       <c r="DT4" t="s">
         <v>120</v>
       </c>
+      <c r="DU4" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -2411,6 +2606,9 @@
       <c r="DT5" t="s">
         <v>120</v>
       </c>
+      <c r="DU5" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -2725,6 +2923,9 @@
       <c r="DT6" t="s">
         <v>120</v>
       </c>
+      <c r="DU6" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -3029,6 +3230,9 @@
       <c r="DT7" t="s">
         <v>120</v>
       </c>
+      <c r="DU7" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -3345,6 +3549,9 @@
       <c r="DT8" t="s">
         <v>120</v>
       </c>
+      <c r="DU8" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -3661,6 +3868,9 @@
       <c r="DT9" t="s">
         <v>120</v>
       </c>
+      <c r="DU9" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -3985,6 +4195,9 @@
       <c r="DT10" t="s">
         <v>120</v>
       </c>
+      <c r="DU10" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -4305,6 +4518,9 @@
       <c r="DT11" t="s">
         <v>120</v>
       </c>
+      <c r="DU11" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -4638,6 +4854,9 @@
       </c>
       <c r="DT12" t="s">
         <v>120</v>
+      </c>
+      <c r="DU12" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="13">
@@ -4957,6 +5176,9 @@
       <c r="DT13" t="s">
         <v>120</v>
       </c>
+      <c r="DU13" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -5266,6 +5488,9 @@
       </c>
       <c r="DT14" t="s">
         <v>120</v>
+      </c>
+      <c r="DU14" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="15">
@@ -5581,6 +5806,9 @@
       <c r="DT15" t="s">
         <v>227</v>
       </c>
+      <c r="DU15" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -5943,6 +6171,9 @@
       <c r="DT16" t="s">
         <v>120</v>
       </c>
+      <c r="DU16" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -6293,6 +6524,9 @@
       <c r="DT17" t="s">
         <v>120</v>
       </c>
+      <c r="DU17" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -6611,7 +6845,7 @@
         <v>229</v>
       </c>
       <c r="DF18" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="DG18" t="s">
         <v>229</v>
@@ -6623,7 +6857,7 @@
         <v>229</v>
       </c>
       <c r="DJ18" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="DK18" t="s">
         <v>229</v>
@@ -6641,10 +6875,10 @@
         <v>229</v>
       </c>
       <c r="DP18" t="s">
+        <v>229</v>
+      </c>
+      <c r="DQ18" t="s">
         <v>233</v>
-      </c>
-      <c r="DQ18" t="s">
-        <v>229</v>
       </c>
       <c r="DR18" t="s">
         <v>229</v>
@@ -6654,6 +6888,9 @@
       </c>
       <c r="DT18" t="s">
         <v>227</v>
+      </c>
+      <c r="DU18" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="19">
@@ -7013,6 +7250,9 @@
       <c r="DT19" t="s">
         <v>120</v>
       </c>
+      <c r="DU19" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -7387,6 +7627,9 @@
       <c r="DT20" t="s">
         <v>120</v>
       </c>
+      <c r="DU20" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -7761,6 +8004,9 @@
       <c r="DT21" t="s">
         <v>227</v>
       </c>
+      <c r="DU21" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -8129,6 +8375,9 @@
       <c r="DT22" t="s">
         <v>227</v>
       </c>
+      <c r="DU22" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -8490,6 +8739,9 @@
       </c>
       <c r="DT23" t="s">
         <v>229</v>
+      </c>
+      <c r="DU23" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="24">
@@ -8823,6 +9075,9 @@
       <c r="DT24" t="s">
         <v>120</v>
       </c>
+      <c r="DU24" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -9184,6 +9439,9 @@
       </c>
       <c r="DT25" t="s">
         <v>227</v>
+      </c>
+      <c r="DU25" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="26">
@@ -9523,6 +9781,9 @@
       <c r="DT26" t="s">
         <v>120</v>
       </c>
+      <c r="DU26" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -9880,6 +10141,9 @@
       </c>
       <c r="DT27" t="s">
         <v>120</v>
+      </c>
+      <c r="DU27" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="28">
@@ -10235,6 +10499,9 @@
       <c r="DT28" t="s">
         <v>120</v>
       </c>
+      <c r="DU28" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
@@ -10536,6 +10803,9 @@
       </c>
       <c r="DT29" t="s">
         <v>229</v>
+      </c>
+      <c r="DU29" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="30">
@@ -10778,7 +11048,7 @@
         <v>229</v>
       </c>
       <c r="DC30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="DD30" t="s">
         <v>229</v>
@@ -10802,7 +11072,7 @@
         <v>230</v>
       </c>
       <c r="DK30" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="DL30" t="s">
         <v>229</v>
@@ -10830,6 +11100,9 @@
       </c>
       <c r="DT30" t="s">
         <v>227</v>
+      </c>
+      <c r="DU30" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="31">
@@ -11119,6 +11392,9 @@
       <c r="DT31" t="s">
         <v>227</v>
       </c>
+      <c r="DU31" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -11481,6 +11757,9 @@
       <c r="DT32" t="s">
         <v>229</v>
       </c>
+      <c r="DU32" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
@@ -11842,6 +12121,9 @@
       </c>
       <c r="DT33" t="s">
         <v>229</v>
+      </c>
+      <c r="DU33" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="34">
@@ -12138,6 +12420,9 @@
       </c>
       <c r="DT34" t="s">
         <v>120</v>
+      </c>
+      <c r="DU34" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="35">
@@ -12431,6 +12716,9 @@
       <c r="DT35" t="s">
         <v>120</v>
       </c>
+      <c r="DU35" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
@@ -12723,6 +13011,9 @@
       <c r="DT36" t="s">
         <v>120</v>
       </c>
+      <c r="DU36" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
@@ -13082,6 +13373,9 @@
       </c>
       <c r="DT37" t="s">
         <v>229</v>
+      </c>
+      <c r="DU37" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="38">
@@ -13425,6 +13719,9 @@
       <c r="DT38" t="s">
         <v>120</v>
       </c>
+      <c r="DU38" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
@@ -13787,6 +14084,9 @@
       <c r="DT39" t="s">
         <v>120</v>
       </c>
+      <c r="DU39" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
@@ -14151,6 +14451,9 @@
       <c r="DT40" t="s">
         <v>120</v>
       </c>
+      <c r="DU40" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
@@ -14512,6 +14815,9 @@
       </c>
       <c r="DT41" t="s">
         <v>120</v>
+      </c>
+      <c r="DU41" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="42">
@@ -14739,10 +15045,10 @@
         <v>216</v>
       </c>
       <c r="CT42" t="s">
+        <v>216</v>
+      </c>
+      <c r="CU42" t="s">
         <v>217</v>
-      </c>
-      <c r="CU42" t="s">
-        <v>216</v>
       </c>
       <c r="CV42" t="s">
         <v>120</v>
@@ -14818,6 +15124,9 @@
       </c>
       <c r="DT42" t="s">
         <v>120</v>
+      </c>
+      <c r="DU42" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="43">
@@ -15159,6 +15468,9 @@
       <c r="DT43" t="s">
         <v>120</v>
       </c>
+      <c r="DU43" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
@@ -15494,6 +15806,9 @@
       </c>
       <c r="DT44" t="s">
         <v>120</v>
+      </c>
+      <c r="DU44" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="45">
@@ -15817,6 +16132,9 @@
       <c r="DT45" t="s">
         <v>120</v>
       </c>
+      <c r="DU45" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
@@ -16135,6 +16453,9 @@
       <c r="DT46" t="s">
         <v>229</v>
       </c>
+      <c r="DU46" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
@@ -16508,6 +16829,9 @@
       </c>
       <c r="DT47" t="s">
         <v>230</v>
+      </c>
+      <c r="DU47" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="48">
@@ -16822,6 +17146,9 @@
       </c>
       <c r="DT48" t="s">
         <v>120</v>
+      </c>
+      <c r="DU48" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="49">
@@ -17141,6 +17468,9 @@
       <c r="DT49" t="s">
         <v>229</v>
       </c>
+      <c r="DU49" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
@@ -17472,6 +17802,9 @@
       </c>
       <c r="DT50" t="s">
         <v>229</v>
+      </c>
+      <c r="DU50" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="51">
@@ -17805,6 +18138,9 @@
       <c r="DT51" t="s">
         <v>229</v>
       </c>
+      <c r="DU51" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
@@ -18166,6 +18502,9 @@
       </c>
       <c r="DT52" t="s">
         <v>231</v>
+      </c>
+      <c r="DU52" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="53">
@@ -18502,6 +18841,9 @@
       </c>
       <c r="DT53" t="s">
         <v>120</v>
+      </c>
+      <c r="DU53" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="54">
@@ -18762,10 +19104,10 @@
         <v>1.0000001192092896</v>
       </c>
       <c r="CS54" t="s">
+        <v>217</v>
+      </c>
+      <c r="CT54" t="s">
         <v>216</v>
-      </c>
-      <c r="CT54" t="s">
-        <v>217</v>
       </c>
       <c r="CU54" t="s">
         <v>120</v>
@@ -18844,6 +19186,9 @@
       </c>
       <c r="DT54" t="s">
         <v>227</v>
+      </c>
+      <c r="DU54" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="55">
@@ -19194,6 +19539,9 @@
       </c>
       <c r="DT55" t="s">
         <v>227</v>
+      </c>
+      <c r="DU55" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="56">
@@ -19541,6 +19889,9 @@
       <c r="DT56" t="s">
         <v>120</v>
       </c>
+      <c r="DU56" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
@@ -19888,6 +20239,9 @@
       </c>
       <c r="DT57" t="s">
         <v>227</v>
+      </c>
+      <c r="DU57" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="58">
@@ -20211,6 +20565,9 @@
       <c r="DT58" t="s">
         <v>229</v>
       </c>
+      <c r="DU58" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
@@ -20509,7 +20866,7 @@
         <v>217</v>
       </c>
       <c r="DB59" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="DC59" t="s">
         <v>229</v>
@@ -20521,7 +20878,7 @@
         <v>229</v>
       </c>
       <c r="DF59" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="DG59" t="s">
         <v>120</v>
@@ -20564,6 +20921,9 @@
       </c>
       <c r="DT59" t="s">
         <v>227</v>
+      </c>
+      <c r="DU59" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="60">
@@ -20842,19 +21202,19 @@
         <v>0.99999994039535522</v>
       </c>
       <c r="CS60" t="s">
+        <v>215</v>
+      </c>
+      <c r="CT60" t="s">
         <v>217</v>
-      </c>
-      <c r="CT60" t="s">
-        <v>215</v>
       </c>
       <c r="CU60" t="s">
         <v>217</v>
       </c>
       <c r="CV60" t="s">
+        <v>217</v>
+      </c>
+      <c r="CW60" t="s">
         <v>215</v>
-      </c>
-      <c r="CW60" t="s">
-        <v>217</v>
       </c>
       <c r="CX60" t="s">
         <v>120</v>
@@ -20875,16 +21235,16 @@
         <v>229</v>
       </c>
       <c r="DD60" t="s">
+        <v>232</v>
+      </c>
+      <c r="DE60" t="s">
+        <v>230</v>
+      </c>
+      <c r="DF60" t="s">
         <v>229</v>
       </c>
-      <c r="DE60" t="s">
+      <c r="DG60" t="s">
         <v>229</v>
-      </c>
-      <c r="DF60" t="s">
-        <v>230</v>
-      </c>
-      <c r="DG60" t="s">
-        <v>230</v>
       </c>
       <c r="DH60" t="s">
         <v>229</v>
@@ -20893,13 +21253,13 @@
         <v>230</v>
       </c>
       <c r="DJ60" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="DK60" t="s">
+        <v>229</v>
+      </c>
+      <c r="DL60" t="s">
         <v>230</v>
-      </c>
-      <c r="DL60" t="s">
-        <v>229</v>
       </c>
       <c r="DM60" t="s">
         <v>120</v>
@@ -20924,6 +21284,9 @@
       </c>
       <c r="DT60" t="s">
         <v>227</v>
+      </c>
+      <c r="DU60" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="61">
@@ -21213,6 +21576,9 @@
       <c r="DT61" t="s">
         <v>233</v>
       </c>
+      <c r="DU61" t="s">
+        <v>313</v>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>